<commit_message>
Add new role as certification manager, other dashboard changes
</commit_message>
<xml_diff>
--- a/db/imports/licence_user_allocation.xlsx
+++ b/db/imports/licence_user_allocation.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3960" uniqueCount="1819">
   <si>
     <t>Name</t>
   </si>
@@ -5495,6 +5495,12 @@
   </si>
   <si>
     <t>GSAS OPERATIONS - CGP</t>
+  </si>
+  <si>
+    <t>a.arshad@gord.qa</t>
+  </si>
+  <si>
+    <t>Anjum Arshad</t>
   </si>
 </sst>
 </file>
@@ -6522,27 +6528,6 @@
     <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6570,6 +6555,9 @@
     <xf numFmtId="0" fontId="22" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6582,17 +6570,23 @@
     <xf numFmtId="0" fontId="23" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="41" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -6606,6 +6600,12 @@
     <xf numFmtId="0" fontId="22" fillId="41" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="43" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -6617,6 +6617,12 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6668,7 +6674,37 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="71">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -31031,41 +31067,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="83" t="s">
         <v>1259</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
     </row>
     <row r="4" spans="1:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="70" t="s">
         <v>1321</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-      <c r="F4" s="80" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="F4" s="73" t="s">
         <v>1274</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="84" t="s">
         <v>1267</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
       <c r="F6" s="23" t="s">
         <v>1278</v>
       </c>
@@ -31111,7 +31147,7 @@
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="75" t="s">
         <v>1289</v>
       </c>
       <c r="G8" s="25" t="s">
@@ -31131,7 +31167,7 @@
       <c r="B9" s="27"/>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
-      <c r="F9" s="83"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="25" t="s">
         <v>1256</v>
       </c>
@@ -31149,7 +31185,7 @@
       <c r="B10" s="27"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39"/>
-      <c r="F10" s="83"/>
+      <c r="F10" s="76"/>
       <c r="G10" s="25" t="s">
         <v>1280</v>
       </c>
@@ -31167,7 +31203,7 @@
       <c r="B11" s="27"/>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
-      <c r="F11" s="83"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="25" t="s">
         <v>1257</v>
       </c>
@@ -31185,7 +31221,7 @@
       <c r="B12" s="27"/>
       <c r="C12" s="38"/>
       <c r="D12" s="39"/>
-      <c r="F12" s="84"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="25" t="s">
         <v>1281</v>
       </c>
@@ -31294,43 +31330,43 @@
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="70" t="s">
         <v>1295</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="79"/>
-      <c r="F19" s="80" t="s">
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="72"/>
+      <c r="F19" s="73" t="s">
         <v>1769</v>
       </c>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
     </row>
     <row r="21" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="88" t="s">
         <v>1261</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="F21" s="71" t="s">
+      <c r="B21" s="88"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="F21" s="78" t="s">
         <v>1293</v>
       </c>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="85"/>
-      <c r="K21" s="86" t="s">
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="79"/>
+      <c r="K21" s="80" t="s">
         <v>1289</v>
       </c>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="88"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="81"/>
+      <c r="N21" s="82"/>
     </row>
     <row r="22" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
@@ -31485,12 +31521,12 @@
       <c r="N28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="84" t="s">
         <v>1246</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
       <c r="F29" s="33" t="s">
         <v>1258</v>
       </c>
@@ -31557,18 +31593,18 @@
       <c r="B32" s="42"/>
       <c r="C32" s="38"/>
       <c r="D32" s="39"/>
-      <c r="F32" s="72" t="s">
+      <c r="F32" s="85" t="s">
         <v>1291</v>
       </c>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="74"/>
-      <c r="K32" s="72" t="s">
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="87"/>
+      <c r="K32" s="85" t="s">
         <v>1290</v>
       </c>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="74"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="87"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
@@ -31657,12 +31693,12 @@
       <c r="N36" s="22"/>
     </row>
     <row r="37" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="84" t="s">
         <v>1269</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
       <c r="F37" s="33" t="s">
         <v>1297</v>
       </c>
@@ -31808,18 +31844,18 @@
       <c r="D44" s="47"/>
     </row>
     <row r="45" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F45" s="71" t="s">
+      <c r="F45" s="78" t="s">
         <v>1282</v>
       </c>
-      <c r="G45" s="71"/>
-      <c r="H45" s="71"/>
-      <c r="I45" s="71"/>
-      <c r="K45" s="71" t="s">
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="78"/>
+      <c r="K45" s="78" t="s">
         <v>1283</v>
       </c>
-      <c r="L45" s="71"/>
-      <c r="M45" s="71"/>
-      <c r="N45" s="71"/>
+      <c r="L45" s="78"/>
+      <c r="M45" s="78"/>
+      <c r="N45" s="78"/>
     </row>
     <row r="46" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F46" s="30"/>
@@ -31957,12 +31993,12 @@
       <c r="F54"/>
     </row>
     <row r="55" spans="6:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F55" s="71" t="s">
+      <c r="F55" s="78" t="s">
         <v>1284</v>
       </c>
-      <c r="G55" s="71"/>
-      <c r="H55" s="71"/>
-      <c r="I55" s="71"/>
+      <c r="G55" s="78"/>
+      <c r="H55" s="78"/>
+      <c r="I55" s="78"/>
     </row>
     <row r="56" spans="6:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F56" s="30"/>
@@ -32042,42 +32078,33 @@
       <c r="F64"/>
     </row>
     <row r="67" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F67" s="76" t="s">
+      <c r="F67" s="69" t="s">
         <v>1768</v>
       </c>
-      <c r="G67" s="76"/>
-      <c r="H67" s="76"/>
-      <c r="I67" s="76"/>
-      <c r="J67" s="76"/>
-      <c r="K67" s="76"/>
-      <c r="L67" s="76"/>
-      <c r="M67" s="76"/>
-      <c r="N67" s="76"/>
+      <c r="G67" s="69"/>
+      <c r="H67" s="69"/>
+      <c r="I67" s="69"/>
+      <c r="J67" s="69"/>
+      <c r="K67" s="69"/>
+      <c r="L67" s="69"/>
+      <c r="M67" s="69"/>
+      <c r="N67" s="69"/>
     </row>
     <row r="68" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F68" s="76" t="s">
+      <c r="F68" s="69" t="s">
         <v>1771</v>
       </c>
-      <c r="G68" s="76"/>
-      <c r="H68" s="76"/>
-      <c r="I68" s="76"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="76"/>
-      <c r="M68" s="76"/>
-      <c r="N68" s="76"/>
+      <c r="G68" s="69"/>
+      <c r="H68" s="69"/>
+      <c r="I68" s="69"/>
+      <c r="J68" s="69"/>
+      <c r="K68" s="69"/>
+      <c r="L68" s="69"/>
+      <c r="M68" s="69"/>
+      <c r="N68" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F68:N68"/>
-    <mergeCell ref="F67:N67"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F19:N19"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="K21:N21"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="F55:I55"/>
@@ -32088,11 +32115,20 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="F45:I45"/>
     <mergeCell ref="K45:N45"/>
+    <mergeCell ref="F68:N68"/>
+    <mergeCell ref="F67:N67"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F19:N19"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="K21:N21"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="A66:A1048576 A44 A1">
-    <cfRule type="duplicateValues" dxfId="67" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -37876,8 +37912,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D35" r:id="rId1"/>
@@ -37889,10 +37925,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39696,15 +39732,71 @@
         <v>517</v>
       </c>
     </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="67" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>37</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F38:F1048576 F1:F36">
-    <cfRule type="duplicateValues" dxfId="63" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="68"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1"/>
+    <hyperlink ref="F37" r:id="rId2" display="mailto:a.arshad@gord.qa"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:a.arshad@gord.qa"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -39731,48 +39823,48 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="83" t="s">
         <v>1301</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="70" t="s">
         <v>1320</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-      <c r="F4" s="77" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="F4" s="70" t="s">
         <v>1295</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="79"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="84" t="s">
         <v>1302</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="F6" s="98" t="s">
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="F6" s="96" t="s">
         <v>1312</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
@@ -39786,11 +39878,11 @@
       <c r="F7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="93" t="s">
         <v>1331</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="97"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="95"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
@@ -39852,11 +39944,11 @@
       <c r="F11" s="25" t="s">
         <v>1322</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="93" t="s">
         <v>1323</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
@@ -39894,11 +39986,11 @@
       <c r="A14" s="25" t="s">
         <v>1243</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="93" t="s">
         <v>1776</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
       <c r="F14" s="25" t="s">
         <v>1319</v>
       </c>
@@ -39914,11 +40006,11 @@
       <c r="A15" s="25" t="s">
         <v>1315</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="93" t="s">
         <v>1777</v>
       </c>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
       <c r="F15" s="25" t="s">
         <v>1332</v>
       </c>
@@ -39949,12 +40041,12 @@
       <c r="D17" s="46" t="s">
         <v>1299</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="F17" s="84" t="s">
         <v>1246</v>
       </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
@@ -39985,12 +40077,12 @@
       <c r="I19" s="57"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="73" t="s">
         <v>1322</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
       <c r="F20" s="25" t="s">
         <v>1251</v>
       </c>
@@ -40008,10 +40100,10 @@
       <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="97" t="s">
         <v>1278</v>
       </c>
-      <c r="B22" s="100"/>
+      <c r="B22" s="98"/>
       <c r="C22" s="30" t="s">
         <v>1276</v>
       </c>
@@ -40028,10 +40120,10 @@
       <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="91" t="s">
         <v>1327</v>
       </c>
-      <c r="B23" s="96"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="26" t="s">
         <v>1328</v>
       </c>
@@ -40048,7 +40140,7 @@
       <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="89" t="s">
         <v>1293</v>
       </c>
       <c r="B24" s="36" t="s">
@@ -40063,7 +40155,7 @@
       <c r="F24"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="94"/>
+      <c r="A25" s="90"/>
       <c r="B25" s="36" t="s">
         <v>1781</v>
       </c>
@@ -40073,15 +40165,15 @@
       <c r="D25" s="44" t="s">
         <v>1299</v>
       </c>
-      <c r="F25" s="70" t="s">
+      <c r="F25" s="84" t="s">
         <v>1269</v>
       </c>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="89" t="s">
         <v>1289</v>
       </c>
       <c r="B26" s="36" t="s">
@@ -40107,7 +40199,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="94"/>
+      <c r="A27" s="90"/>
       <c r="B27" s="36" t="s">
         <v>1781</v>
       </c>
@@ -40131,7 +40223,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="93" t="s">
+      <c r="A28" s="89" t="s">
         <v>1291</v>
       </c>
       <c r="B28" s="36" t="s">
@@ -40151,7 +40243,7 @@
       <c r="I28" s="26"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="94"/>
+      <c r="A29" s="90"/>
       <c r="B29" s="36" t="s">
         <v>1781</v>
       </c>
@@ -40169,7 +40261,7 @@
       <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="99" t="s">
         <v>1290</v>
       </c>
       <c r="B30" s="36" t="s">
@@ -40185,7 +40277,7 @@
       <c r="I30" s="61"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="89"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="36" t="s">
         <v>1782</v>
       </c>
@@ -40197,7 +40289,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="54" t="s">
         <v>1783</v>
       </c>
@@ -40209,7 +40301,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="89"/>
+      <c r="A33" s="99"/>
       <c r="B33" s="54" t="s">
         <v>1784</v>
       </c>
@@ -40229,10 +40321,10 @@
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="100" t="s">
         <v>1778</v>
       </c>
-      <c r="B34" s="90"/>
+      <c r="B34" s="100"/>
       <c r="C34" s="26" t="s">
         <v>1328</v>
       </c>
@@ -40241,10 +40333,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="100" t="s">
         <v>1779</v>
       </c>
-      <c r="B35" s="90"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="26" t="s">
         <v>1328</v>
       </c>
@@ -40253,10 +40345,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="100" t="s">
         <v>1785</v>
       </c>
-      <c r="B36" s="90"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="26" t="s">
         <v>1328</v>
       </c>
@@ -40300,6 +40392,13 @@
     <row r="71" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A28:A29"/>
@@ -40314,18 +40413,11 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="F33 A71:A1048576">
-    <cfRule type="duplicateValues" dxfId="62" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="61" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -56803,225 +56895,225 @@
     <mergeCell ref="AB190:AB191"/>
   </mergeCells>
   <conditionalFormatting sqref="XEZ269:XFB269">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="XEZ295:XFB298">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="XEZ268:XFB268">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="XEZ286:XFB286">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3 B109:B230 B304:B1048576">
-    <cfRule type="duplicateValues" dxfId="56" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="55" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V20">
-    <cfRule type="duplicateValues" dxfId="54" priority="53" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="53" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B26">
-    <cfRule type="duplicateValues" dxfId="53" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21:V29">
-    <cfRule type="duplicateValues" dxfId="52" priority="51" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="51" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30">
-    <cfRule type="duplicateValues" dxfId="51" priority="50" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="50" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V38">
-    <cfRule type="duplicateValues" dxfId="50" priority="49" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="49" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B37">
-    <cfRule type="duplicateValues" dxfId="49" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38:B51">
-    <cfRule type="duplicateValues" dxfId="48" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="45" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39:V51">
-    <cfRule type="duplicateValues" dxfId="45" priority="44" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="44" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B62">
-    <cfRule type="duplicateValues" dxfId="44" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B62">
-    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="42" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B67">
-    <cfRule type="duplicateValues" dxfId="42" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B67">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="duplicateValues" dxfId="40" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69:B71">
-    <cfRule type="duplicateValues" dxfId="38" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69:B71">
-    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B73">
-    <cfRule type="duplicateValues" dxfId="36" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B73">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74:B75">
-    <cfRule type="duplicateValues" dxfId="34" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74:B75">
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B80">
-    <cfRule type="duplicateValues" dxfId="32" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B80">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:B88">
-    <cfRule type="duplicateValues" dxfId="30" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:B88">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89:B90">
-    <cfRule type="duplicateValues" dxfId="28" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89:B90">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:B92">
-    <cfRule type="duplicateValues" dxfId="26" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:B92">
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93:B100">
-    <cfRule type="duplicateValues" dxfId="24" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93:B100">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105 B107">
-    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105 B107">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B102 B104 B106 B108">
-    <cfRule type="duplicateValues" dxfId="20" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B102 B104 B106 B108">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"Expired"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B231:B236">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B237">
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B238">
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B239:B244">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B245">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B246:B248">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B249:B251">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B252:B257">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B258:B268">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B269:B286">
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B287:B288">
-    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B289:B303">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A197:A303">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A189">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A191:A196">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E3 D5:E1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E4">
-    <cfRule type="duplicateValues" dxfId="2" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C145" r:id="rId1"/>

</xml_diff>